<commit_message>
GUIAS DE USO SGCM / ACTUALIZACIÓN DE GUIAS DE USUARIO
</commit_message>
<xml_diff>
--- a/SIEDNL (PDR)/13 MATRIZ DE PRUEBAS/Matriz de Pruebas/Matiz de Pruebas SIEDNL - MIR - Actualizada.xlsx
+++ b/SIEDNL (PDR)/13 MATRIZ DE PRUEBAS/Matriz de Pruebas/Matiz de Pruebas SIEDNL - MIR - Actualizada.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\github\All-documents\SIEDNL (PDR)\ENTREGABLES\Matriz de Pruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\github\All-documents\SIEDNL (PDR)\13 MATRIZ DE PRUEBAS\Matriz de Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -265,9 +265,6 @@
     <t>PBR (SIEDNL)</t>
   </si>
   <si>
-    <t>http://10.200.4.165/</t>
-  </si>
-  <si>
     <t xml:space="preserve">Notificaciones </t>
   </si>
   <si>
@@ -530,6 +527,9 @@
   </si>
   <si>
     <t>airis</t>
+  </si>
+  <si>
+    <t>https://tesoreria-virtual.nl.gob.mx/</t>
   </si>
 </sst>
 </file>
@@ -874,6 +874,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -925,9 +928,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% - Énfasis3" xfId="2" builtinId="40"/>
@@ -935,9 +935,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -949,6 +946,9 @@
     </dxf>
     <dxf>
       <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1023,7 +1023,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Matiz de Pruebas SIEDNL - MIR - copia.xlsx]GRAFICOS!Tabla dinámica1</c:name>
+    <c:name>[Matiz de Pruebas SIEDNL - MIR - Actualizada.xlsx]GRAFICOS!Tabla dinámica1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1058,6 +1058,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1836,6 +1837,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -1937,7 +1939,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Matiz de Pruebas SIEDNL - MIR - copia.xlsx]GRAFICOS!Tabla dinámica2</c:name>
+    <c:name>[Matiz de Pruebas SIEDNL - MIR - Actualizada.xlsx]GRAFICOS!Tabla dinámica2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1967,6 +1969,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2264,6 +2267,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2354,7 +2358,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Matiz de Pruebas SIEDNL - MIR - copia.xlsx]GRAFICOS!Tabla dinámica3</c:name>
+    <c:name>[Matiz de Pruebas SIEDNL - MIR - Actualizada.xlsx]GRAFICOS!Tabla dinámica3</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -2384,6 +2388,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3143,6 +3148,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9794,6 +9800,197 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
+  <location ref="A24:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="11">
+        <item h="1" x="0"/>
+        <item m="1" x="9"/>
+        <item m="1" x="5"/>
+        <item m="1" x="6"/>
+        <item m="1" x="4"/>
+        <item m="1" x="7"/>
+        <item m="1" x="8"/>
+        <item m="1" x="3"/>
+        <item m="1" x="2"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="11"/>
+  </rowFields>
+  <rowItems count="1">
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Cuenta de N° Caso" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Cuenta de N° Caso" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="5">
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A47:B49" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
@@ -9973,197 +10170,6 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
-  <location ref="A24:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="14">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="11">
-        <item h="1" x="0"/>
-        <item m="1" x="9"/>
-        <item m="1" x="5"/>
-        <item m="1" x="6"/>
-        <item m="1" x="4"/>
-        <item m="1" x="7"/>
-        <item m="1" x="8"/>
-        <item m="1" x="3"/>
-        <item m="1" x="2"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="11"/>
-  </rowFields>
-  <rowItems count="1">
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Cuenta de N° Caso" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="1">
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
-  <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="14">
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Cuenta de N° Caso" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="5">
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A6:N262" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" headerRowCellStyle="60% - Énfasis3">
   <autoFilter ref="A6:N262"/>
@@ -10172,12 +10178,12 @@
     <tableColumn id="2" name="Menús" dataDxfId="5"/>
     <tableColumn id="3" name="Submenú"/>
     <tableColumn id="4" name="Perfil"/>
-    <tableColumn id="5" name="Usuario " dataDxfId="0"/>
-    <tableColumn id="6" name="Acción" dataDxfId="4"/>
+    <tableColumn id="5" name="Usuario " dataDxfId="4"/>
+    <tableColumn id="6" name="Acción" dataDxfId="3"/>
     <tableColumn id="7" name="Estatus de Prueba"/>
-    <tableColumn id="8" name="Resultado Obtenido" dataDxfId="3"/>
-    <tableColumn id="9" name="Resultado Esperado" dataDxfId="2"/>
-    <tableColumn id="10" name="N° de Indicente" dataDxfId="1"/>
+    <tableColumn id="8" name="Resultado Obtenido" dataDxfId="2"/>
+    <tableColumn id="9" name="Resultado Esperado" dataDxfId="1"/>
+    <tableColumn id="10" name="N° de Indicente" dataDxfId="0"/>
     <tableColumn id="11" name="Desarrollador"/>
     <tableColumn id="12" name="Estatus Incidente"/>
     <tableColumn id="13" name="N° de Tarea Jira"/>
@@ -10435,9 +10441,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:N285"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F80" sqref="F80"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -10459,94 +10465,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
     </row>
     <row r="3" spans="1:14" s="20" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="27" t="s">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
     </row>
     <row r="4" spans="1:14" s="20" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
     </row>
     <row r="5" spans="1:14" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="37"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
     </row>
     <row r="6" spans="1:14" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
@@ -10561,7 +10567,7 @@
       <c r="D6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="40" t="s">
+      <c r="E6" s="23" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="22" t="s">
@@ -10600,13 +10606,13 @@
         <v>43</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>46</v>
@@ -10624,13 +10630,13 @@
         <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>48</v>
@@ -10645,16 +10651,16 @@
         <v>3</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>35</v>
@@ -10672,13 +10678,13 @@
         <v>45</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>18</v>
@@ -10693,16 +10699,16 @@
         <v>45</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>135</v>
-      </c>
-      <c r="D11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>136</v>
       </c>
       <c r="N11" s="1"/>
     </row>
@@ -10714,13 +10720,13 @@
         <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>20</v>
@@ -10738,16 +10744,16 @@
         <v>45</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N13" s="1"/>
     </row>
@@ -10759,19 +10765,19 @@
         <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N14" s="1"/>
     </row>
@@ -10783,19 +10789,19 @@
         <v>45</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N15" s="1"/>
     </row>
@@ -10804,22 +10810,22 @@
         <v>10</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D16" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="I16" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N16" s="1"/>
     </row>
@@ -10828,19 +10834,19 @@
         <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>22</v>
@@ -10852,19 +10858,19 @@
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>22</v>
@@ -10876,22 +10882,22 @@
         <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N19" s="1"/>
     </row>
@@ -10900,22 +10906,22 @@
         <v>16</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="N20" s="1"/>
     </row>
@@ -10924,22 +10930,22 @@
         <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F21" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="N21" s="1"/>
     </row>
@@ -10948,22 +10954,22 @@
         <v>18</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F22" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="N22" s="1"/>
     </row>
@@ -10972,22 +10978,22 @@
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F23" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="N23" s="1"/>
     </row>
@@ -10996,22 +11002,22 @@
         <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="N24" s="1"/>
     </row>
@@ -11020,22 +11026,22 @@
         <v>21</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N25" s="1"/>
     </row>
@@ -11044,29 +11050,29 @@
         <v>22</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D26" t="s">
-        <v>76</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="I26" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N27" s="1"/>
     </row>
@@ -11075,22 +11081,22 @@
         <v>23</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F28" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" t="s">
         <v>74</v>
-      </c>
-      <c r="I28" t="s">
-        <v>75</v>
       </c>
       <c r="N28" s="1"/>
     </row>
@@ -11099,22 +11105,22 @@
         <v>24</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F29" t="s">
+        <v>66</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F29" t="s">
-        <v>67</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="N29" s="1"/>
     </row>
@@ -11123,22 +11129,22 @@
         <v>25</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J30"/>
       <c r="N30" s="1"/>
@@ -11148,22 +11154,22 @@
         <v>26</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J31"/>
       <c r="N31" s="1"/>
@@ -11173,22 +11179,22 @@
         <v>27</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N32" s="1"/>
     </row>
@@ -11197,22 +11203,22 @@
         <v>28</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N33" s="1"/>
     </row>
@@ -11221,22 +11227,22 @@
         <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" t="s">
         <v>82</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="I34" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N34" s="1"/>
     </row>
@@ -11245,19 +11251,19 @@
         <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" t="s">
         <v>82</v>
       </c>
-      <c r="D35" t="s">
-        <v>83</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>22</v>
@@ -11269,19 +11275,19 @@
         <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" t="s">
         <v>82</v>
       </c>
-      <c r="D36" t="s">
-        <v>83</v>
-      </c>
       <c r="E36" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>22</v>
@@ -11293,22 +11299,22 @@
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" t="s">
         <v>82</v>
       </c>
-      <c r="D37" t="s">
-        <v>83</v>
-      </c>
       <c r="E37" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N37" s="1"/>
     </row>
@@ -11317,22 +11323,22 @@
         <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" t="s">
         <v>82</v>
       </c>
-      <c r="D38" t="s">
-        <v>83</v>
-      </c>
       <c r="E38" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N38" s="1"/>
     </row>
@@ -11341,22 +11347,22 @@
         <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" t="s">
         <v>82</v>
       </c>
-      <c r="D39" t="s">
-        <v>83</v>
-      </c>
       <c r="E39" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N39" s="1"/>
     </row>
@@ -11365,22 +11371,22 @@
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N40" s="1"/>
     </row>
@@ -11389,22 +11395,22 @@
         <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F41" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I41" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="N41" s="1"/>
     </row>
@@ -11413,22 +11419,22 @@
         <v>37</v>
       </c>
       <c r="B42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F42" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I42" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="N42" s="1"/>
     </row>
@@ -11437,22 +11443,22 @@
         <v>38</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F43" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I43" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="N43" s="1"/>
     </row>
@@ -11461,22 +11467,22 @@
         <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F44" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I44" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="N44" s="1"/>
     </row>
@@ -11485,22 +11491,22 @@
         <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N45" s="1"/>
     </row>
@@ -11509,22 +11515,22 @@
         <v>41</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N46" s="1"/>
     </row>
@@ -11533,22 +11539,22 @@
         <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N47" s="1"/>
     </row>
@@ -11557,22 +11563,22 @@
         <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N48" s="1"/>
     </row>
@@ -11581,22 +11587,22 @@
         <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N49" s="1"/>
     </row>
@@ -11605,22 +11611,22 @@
         <v>45</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
@@ -11628,22 +11634,22 @@
         <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
@@ -11651,22 +11657,22 @@
         <v>47</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N52" s="1"/>
     </row>
@@ -11675,22 +11681,22 @@
         <v>48</v>
       </c>
       <c r="B53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N53" s="1"/>
     </row>
@@ -11699,22 +11705,22 @@
         <v>49</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N54" s="1"/>
     </row>
@@ -11723,19 +11729,19 @@
         <v>50</v>
       </c>
       <c r="B55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D55" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I55" s="3" t="s">
         <v>22</v>
@@ -11747,19 +11753,19 @@
         <v>51</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>22</v>
@@ -11771,22 +11777,22 @@
         <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N57" s="1"/>
     </row>
@@ -11795,22 +11801,22 @@
         <v>53</v>
       </c>
       <c r="B58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D58" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N58" s="1"/>
     </row>
@@ -11819,22 +11825,22 @@
         <v>54</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D59" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N59" s="1"/>
     </row>
@@ -11843,22 +11849,22 @@
         <v>55</v>
       </c>
       <c r="B60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D60" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N60" s="1"/>
     </row>
@@ -11867,22 +11873,22 @@
         <v>56</v>
       </c>
       <c r="B61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D61" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F61" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I61" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="I61" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="N61" s="1"/>
     </row>
@@ -11891,22 +11897,22 @@
         <v>57</v>
       </c>
       <c r="B62" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F62" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I62" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="N62" s="1"/>
     </row>
@@ -11915,22 +11921,22 @@
         <v>58</v>
       </c>
       <c r="B63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D63" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F63" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I63" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="N63" s="1"/>
     </row>
@@ -11939,22 +11945,22 @@
         <v>59</v>
       </c>
       <c r="B64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D64" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F64" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I64" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="I64" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="N64" s="1"/>
     </row>
@@ -11963,22 +11969,22 @@
         <v>60</v>
       </c>
       <c r="B65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D65" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F65" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I65" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="N65" s="1"/>
     </row>
@@ -11987,22 +11993,22 @@
         <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N66" s="1"/>
     </row>
@@ -12011,22 +12017,22 @@
         <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C67" t="s">
+        <v>63</v>
+      </c>
+      <c r="D67" t="s">
+        <v>90</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D67" t="s">
-        <v>91</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="I67" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N67" s="1"/>
     </row>
@@ -12035,22 +12041,22 @@
         <v>63</v>
       </c>
       <c r="B68" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D68" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N68" s="1"/>
     </row>
@@ -12059,22 +12065,22 @@
         <v>64</v>
       </c>
       <c r="B69" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C69" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D69" t="s">
+        <v>90</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E69" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F69" s="3" t="s">
+      <c r="I69" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="I69" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="N69" s="1"/>
     </row>
@@ -12083,22 +12089,22 @@
         <v>65</v>
       </c>
       <c r="B70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C70" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D70" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N70" s="1"/>
     </row>
@@ -12107,22 +12113,22 @@
         <v>66</v>
       </c>
       <c r="B71" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D71" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F71" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N71" s="1"/>
     </row>
@@ -12131,22 +12137,22 @@
         <v>67</v>
       </c>
       <c r="B72" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C72" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D72" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N72" s="1"/>
     </row>
@@ -12155,22 +12161,22 @@
         <v>68</v>
       </c>
       <c r="B73" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N73" s="1"/>
     </row>
@@ -12179,22 +12185,22 @@
         <v>69</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D74" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N74" s="1"/>
     </row>
@@ -12203,16 +12209,16 @@
         <v>70</v>
       </c>
       <c r="D75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F75" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I75" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="I75" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="L75" t="s">
         <v>39</v>
@@ -13108,57 +13114,57 @@
         <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>